<commit_message>
created docker text file
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="git commands" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -466,28 +464,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>